<commit_message>
Start on ECU code, modify TPS and update can bus messages
-start ECU code
-move canMsg initialisation out of setup()
-added TODOs
-modify some messages in can bus messages.xlsx
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="853" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF02A23A-089E-43A6-B883-D98A78DD2876}"/>
+  <xr:revisionPtr revIDLastSave="874" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63CCD26C-9A82-4320-8E9E-EEDEFBC30116}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25920" yWindow="6240" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="185">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -500,9 +500,6 @@
     <t>Long Description / Functions</t>
   </si>
   <si>
-    <t>Boost: 0: normal 255: boost</t>
-  </si>
-  <si>
     <t>FW Status</t>
   </si>
   <si>
@@ -530,9 +527,6 @@
     <t>Battery voltage(V) = (B1 *256 + B0)*0.1</t>
   </si>
   <si>
-    <t>brake percent (%); 0-100%. Could be calculated based on pressure</t>
-  </si>
-  <si>
     <t>Wheel speed (RPM) = (B1*256 + B0)*0.03; 0-1966RPM</t>
   </si>
   <si>
@@ -557,9 +551,6 @@
     <t>fade (0: fade, 1: immediately change)</t>
   </si>
   <si>
-    <t>angle = (B1*256 + B0)/10 - 180; 0-360</t>
-  </si>
-  <si>
     <t>Front-Rear Differnetial Balance</t>
   </si>
   <si>
@@ -594,6 +585,24 @@
   </si>
   <si>
     <t>12V voltage(V) = B2/10</t>
+  </si>
+  <si>
+    <t>Reverse/Boost</t>
+  </si>
+  <si>
+    <t>Reverse (0:forward, 1:reverse)</t>
+  </si>
+  <si>
+    <t>mode (0: normal 1:eco 2:boost)</t>
+  </si>
+  <si>
+    <t>when changed</t>
+  </si>
+  <si>
+    <t>brake percent (%) B4*0.4; 0-100%. Could be calculated based on pressure</t>
+  </si>
+  <si>
+    <t>angle = (B1*256 + B0)/10 - 180; =180 - 180</t>
   </si>
 </sst>
 </file>
@@ -776,13 +785,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1090,7 +1099,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="R40" sqref="R40"/>
+      <selection pane="bottomLeft" activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,17 +1125,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="9" t="s">
         <v>55</v>
       </c>
@@ -1270,7 +1279,7 @@
         <v>22</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
@@ -1298,7 +1307,7 @@
         <v>22</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="19" t="s">
@@ -1324,7 +1333,7 @@
         <v>22</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="19" t="s">
@@ -1350,7 +1359,7 @@
         <v>22</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="19" t="s">
@@ -1364,16 +1373,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="E14" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="M14" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19" t="s">
@@ -1385,7 +1397,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>137</v>
@@ -1397,7 +1409,7 @@
         <v>22</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P15" s="19" t="s">
         <v>136</v>
@@ -1413,7 +1425,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>4</v>
@@ -1422,7 +1434,7 @@
         <v>22</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P17" s="19" t="s">
         <v>136</v>
@@ -1433,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>4</v>
@@ -1442,7 +1454,7 @@
         <v>22</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P18" s="19" t="s">
         <v>136</v>
@@ -1453,13 +1465,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P19" s="19" t="s">
         <v>136</v>
@@ -1470,13 +1482,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P20" s="19" t="s">
         <v>136</v>
@@ -1487,13 +1499,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P21" s="19" t="s">
         <v>136</v>
@@ -1585,13 +1597,13 @@
         <v>61</v>
       </c>
       <c r="P34" t="s">
+        <v>155</v>
+      </c>
+      <c r="R34" t="s">
         <v>156</v>
       </c>
-      <c r="R34" t="s">
-        <v>157</v>
-      </c>
       <c r="T34" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1639,6 +1651,30 @@
       <c r="B36">
         <v>34</v>
       </c>
+      <c r="C36" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="P36" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B37">
@@ -1665,11 +1701,11 @@
         <v>57</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26" t="s">
@@ -1689,7 +1725,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
@@ -1698,13 +1734,13 @@
         <v>22</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="P39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Q39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
@@ -1759,7 +1795,7 @@
         <v>61</v>
       </c>
       <c r="P46" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="R46" t="s">
         <v>98</v>
@@ -1786,16 +1822,13 @@
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>17</v>
-      </c>
-      <c r="F50" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -1817,12 +1850,6 @@
       </c>
       <c r="S50" t="s">
         <v>102</v>
-      </c>
-      <c r="T50" t="s">
-        <v>163</v>
-      </c>
-      <c r="U50" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1905,11 +1932,11 @@
         <v>61</v>
       </c>
       <c r="P54" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="Q54" s="26"/>
       <c r="R54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
@@ -1930,7 +1957,7 @@
       </c>
       <c r="Q55" s="26"/>
       <c r="R55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
@@ -1951,7 +1978,7 @@
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
@@ -1972,7 +1999,7 @@
       </c>
       <c r="Q57" s="26"/>
       <c r="R57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
@@ -1992,11 +2019,11 @@
         <v>57</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q58" s="26"/>
       <c r="R58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
@@ -2019,10 +2046,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -2031,13 +2058,13 @@
         <v>22</v>
       </c>
       <c r="N62" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="P62" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q62" t="s">
         <v>173</v>
-      </c>
-      <c r="P62" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.25">
@@ -2045,10 +2072,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -2057,13 +2084,13 @@
         <v>22</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P63" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Q63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
@@ -2128,18 +2155,18 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="27" t="s">
+      <c r="P67" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27" t="s">
+      <c r="Q67" s="25"/>
+      <c r="R67" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="S67" s="27"/>
-      <c r="T67" s="27" t="s">
+      <c r="S67" s="25"/>
+      <c r="T67" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="U67" s="27"/>
+      <c r="U67" s="25"/>
       <c r="AB67" s="17" t="s">
         <v>123</v>
       </c>
@@ -2157,18 +2184,18 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="27" t="s">
+      <c r="P68" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="27" t="s">
+      <c r="Q68" s="25"/>
+      <c r="R68" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="S68" s="27"/>
-      <c r="T68" s="27" t="s">
+      <c r="S68" s="25"/>
+      <c r="T68" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="U68" s="27"/>
+      <c r="U68" s="25"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2184,18 +2211,18 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="27" t="s">
+      <c r="P69" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="27" t="s">
+      <c r="Q69" s="25"/>
+      <c r="R69" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="S69" s="27"/>
-      <c r="T69" s="27" t="s">
+      <c r="S69" s="25"/>
+      <c r="T69" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="U69" s="27"/>
+      <c r="U69" s="25"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -2423,7 +2450,7 @@
         <v>106</v>
       </c>
       <c r="S98" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T98" s="12" t="s">
         <v>107</v>
@@ -2455,7 +2482,7 @@
         <v>106</v>
       </c>
       <c r="S99" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="T99" s="12" t="s">
         <v>107</v>
@@ -2493,7 +2520,7 @@
         <v>106</v>
       </c>
       <c r="S101" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -3502,6 +3529,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3509,17 +3547,6 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Work on ECU code
ecu code compiles now. No chance to test it though because no access to arduino and CANbus
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="874" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63CCD26C-9A82-4320-8E9E-EEDEFBC30116}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF3F0B7F-833A-4FD2-A0E3-6E2149FC8F95}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="6240" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="186">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -551,9 +551,6 @@
     <t>fade (0: fade, 1: immediately change)</t>
   </si>
   <si>
-    <t>Front-Rear Differnetial Balance</t>
-  </si>
-  <si>
     <t>0: 100%front, 127: 50-50, 255: 100% rear</t>
   </si>
   <si>
@@ -603,6 +600,12 @@
   </si>
   <si>
     <t>angle = (B1*256 + B0)/10 - 180; =180 - 180</t>
+  </si>
+  <si>
+    <t>0 =  error, 1 = ok, 2 = estop pressed, 255 = offline</t>
+  </si>
+  <si>
+    <t>Front-Rear Differential Balance</t>
   </si>
 </sst>
 </file>
@@ -785,13 +788,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1096,10 +1099,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P46" sqref="P46"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,17 +1128,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
       <c r="N1" s="9" t="s">
         <v>55</v>
       </c>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="AB10" s="22" t="s">
         <v>127</v>
@@ -1603,7 +1606,7 @@
         <v>156</v>
       </c>
       <c r="T34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1652,10 +1655,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>137</v>
@@ -1667,13 +1670,13 @@
         <v>20</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P36" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q36" t="s">
         <v>180</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -1725,7 +1728,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
@@ -1734,13 +1737,13 @@
         <v>22</v>
       </c>
       <c r="N39" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="P39" t="s">
         <v>176</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>177</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>178</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
@@ -1795,7 +1798,7 @@
         <v>61</v>
       </c>
       <c r="P46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R46" t="s">
         <v>98</v>
@@ -2046,10 +2049,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -2058,13 +2061,13 @@
         <v>22</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P62" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q62" t="s">
         <v>172</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.25">
@@ -2072,10 +2075,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -2084,13 +2087,13 @@
         <v>22</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
@@ -2155,18 +2158,18 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="25" t="s">
+      <c r="P67" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="Q67" s="25"/>
-      <c r="R67" s="25" t="s">
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S67" s="25"/>
-      <c r="T67" s="25" t="s">
+      <c r="S67" s="27"/>
+      <c r="T67" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="U67" s="25"/>
+      <c r="U67" s="27"/>
       <c r="AB67" s="17" t="s">
         <v>123</v>
       </c>
@@ -2184,18 +2187,18 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="25" t="s">
+      <c r="P68" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25" t="s">
+      <c r="Q68" s="27"/>
+      <c r="R68" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25" t="s">
+      <c r="S68" s="27"/>
+      <c r="T68" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="U68" s="25"/>
+      <c r="U68" s="27"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2211,18 +2214,18 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="25" t="s">
+      <c r="P69" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="Q69" s="25"/>
-      <c r="R69" s="25" t="s">
+      <c r="Q69" s="27"/>
+      <c r="R69" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="S69" s="25"/>
-      <c r="T69" s="25" t="s">
+      <c r="S69" s="27"/>
+      <c r="T69" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="U69" s="25"/>
+      <c r="U69" s="27"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -3529,17 +3532,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3547,6 +3539,17 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Update code for nodes
- BMS has 5v and 12v voltage sensing abilities now
- TPS filter has been improved (still not implemented dual sensors yet)
- Brake message and voltage message in CAN Bus Messages excel updated
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="876" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF3F0B7F-833A-4FD2-A0E3-6E2149FC8F95}"/>
+  <xr:revisionPtr revIDLastSave="893" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D478FF7-B434-45E2-9A30-4D0B0C3F58BA}"/>
   <bookViews>
     <workbookView xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="188">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -518,9 +518,6 @@
     <t>Throttle Position = B0*0.4; 0-100%</t>
   </si>
   <si>
-    <t>Brake Pressure(kPa) = B2 * 4; 0-1000kPa</t>
-  </si>
-  <si>
     <t>Battery Current(A) = -320 + (B3*256 + B2)*0.1</t>
   </si>
   <si>
@@ -578,12 +575,6 @@
     <t>500ms</t>
   </si>
   <si>
-    <t>5V voltage(V) = B1/20</t>
-  </si>
-  <si>
-    <t>12V voltage(V) = B2/10</t>
-  </si>
-  <si>
     <t>Reverse/Boost</t>
   </si>
   <si>
@@ -606,6 +597,21 @@
   </si>
   <si>
     <t>Front-Rear Differential Balance</t>
+  </si>
+  <si>
+    <t>5V voltage(V) = B1/20 SCALING FACTOR MAY CHANGE</t>
+  </si>
+  <si>
+    <t>12V voltage(V) = B2/10 SCALING FACTOR MAY CHANGE</t>
+  </si>
+  <si>
+    <t>0 (reserved)</t>
+  </si>
+  <si>
+    <t>Rear Brake Pressure(kPa) = B2 * 4; 0-1000kPa. If B3 is empty it is the default brake pressure. If B3 is populated it is the front brake pressure</t>
+  </si>
+  <si>
+    <t>Brake Pressure(kPa) = B2 * 4; 0-1000kPa. If B3 is set as 255, B2 is the default brake pressure. If B3 is populated, B2 is the front brake pressure</t>
   </si>
 </sst>
 </file>
@@ -788,13 +794,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1100,9 +1106,9 @@
   <dimension ref="A1:AD301"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,17 +1134,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="9" t="s">
         <v>55</v>
       </c>
@@ -1286,7 +1292,7 @@
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AB10" s="22" t="s">
         <v>127</v>
@@ -1376,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>69</v>
@@ -1468,7 +1474,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>22</v>
@@ -1485,7 +1491,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>22</v>
@@ -1502,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>22</v>
@@ -1602,11 +1608,17 @@
       <c r="P34" t="s">
         <v>155</v>
       </c>
+      <c r="Q34" t="s">
+        <v>185</v>
+      </c>
       <c r="R34" t="s">
-        <v>156</v>
+        <v>187</v>
+      </c>
+      <c r="S34" t="s">
+        <v>186</v>
       </c>
       <c r="T34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1655,10 +1667,10 @@
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>137</v>
@@ -1670,13 +1682,13 @@
         <v>20</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P36" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q36" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -1704,11 +1716,11 @@
         <v>57</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26" t="s">
@@ -1728,7 +1740,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
@@ -1737,13 +1749,19 @@
         <v>22</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P39" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="Q39" t="s">
-        <v>177</v>
+        <v>185</v>
+      </c>
+      <c r="R39" t="s">
+        <v>184</v>
+      </c>
+      <c r="S39" t="s">
+        <v>185</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
@@ -1798,7 +1816,7 @@
         <v>61</v>
       </c>
       <c r="P46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="R46" t="s">
         <v>98</v>
@@ -1935,11 +1953,11 @@
         <v>61</v>
       </c>
       <c r="P54" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q54" s="26"/>
       <c r="R54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
@@ -1960,7 +1978,7 @@
       </c>
       <c r="Q55" s="26"/>
       <c r="R55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
@@ -1981,7 +1999,7 @@
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
@@ -2002,7 +2020,7 @@
       </c>
       <c r="Q57" s="26"/>
       <c r="R57" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
@@ -2022,11 +2040,11 @@
         <v>57</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q58" s="26"/>
       <c r="R58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
@@ -2049,10 +2067,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -2061,13 +2079,13 @@
         <v>22</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P62" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q62" t="s">
         <v>171</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.25">
@@ -2075,10 +2093,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -2087,13 +2105,13 @@
         <v>22</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
@@ -2158,18 +2176,18 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="27" t="s">
+      <c r="P67" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27" t="s">
+      <c r="Q67" s="25"/>
+      <c r="R67" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="S67" s="27"/>
-      <c r="T67" s="27" t="s">
+      <c r="S67" s="25"/>
+      <c r="T67" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="U67" s="27"/>
+      <c r="U67" s="25"/>
       <c r="AB67" s="17" t="s">
         <v>123</v>
       </c>
@@ -2187,18 +2205,18 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="27" t="s">
+      <c r="P68" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="27" t="s">
+      <c r="Q68" s="25"/>
+      <c r="R68" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="S68" s="27"/>
-      <c r="T68" s="27" t="s">
+      <c r="S68" s="25"/>
+      <c r="T68" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="U68" s="27"/>
+      <c r="U68" s="25"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2214,18 +2232,18 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="27" t="s">
+      <c r="P69" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="27" t="s">
+      <c r="Q69" s="25"/>
+      <c r="R69" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="S69" s="27"/>
-      <c r="T69" s="27" t="s">
+      <c r="S69" s="25"/>
+      <c r="T69" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="U69" s="27"/>
+      <c r="U69" s="25"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -2453,7 +2471,7 @@
         <v>106</v>
       </c>
       <c r="S98" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T98" s="12" t="s">
         <v>107</v>
@@ -2485,7 +2503,7 @@
         <v>106</v>
       </c>
       <c r="S99" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T99" s="12" t="s">
         <v>107</v>
@@ -2523,7 +2541,7 @@
         <v>106</v>
       </c>
       <c r="S101" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -3532,6 +3550,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3539,17 +3568,6 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
update SAS code. Add steering calibration function into canbus messages
tested with steering rack and sensor. Not yet tested with CAN Bus
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="893" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D478FF7-B434-45E2-9A30-4D0B0C3F58BA}"/>
+  <xr:revisionPtr revIDLastSave="932" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F12152C5-A2FE-4C6A-AC24-DA56135F7265}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="193">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -330,9 +330,6 @@
   </si>
   <si>
     <t>Batt SOC (%) ;0-100%</t>
-  </si>
-  <si>
-    <t>pending testing with the sensor</t>
   </si>
   <si>
     <t>FL: 0.4%/bit 0-100%</t>
@@ -590,9 +587,6 @@
     <t>brake percent (%) B4*0.4; 0-100%. Could be calculated based on pressure</t>
   </si>
   <si>
-    <t>angle = (B1*256 + B0)/10 - 180; =180 - 180</t>
-  </si>
-  <si>
     <t>0 =  error, 1 = ok, 2 = estop pressed, 255 = offline</t>
   </si>
   <si>
@@ -612,6 +606,32 @@
   </si>
   <si>
     <t>Brake Pressure(kPa) = B2 * 4; 0-1000kPa. If B3 is set as 255, B2 is the default brake pressure. If B3 is populated, B2 is the front brake pressure</t>
+  </si>
+  <si>
+    <t>Calibrate Steering</t>
+  </si>
+  <si>
+    <t>HUD/SAS</t>
+  </si>
+  <si>
+    <t>angle(degrees) = ((B1*256 + B0)-2048)/130degrees
+raw data is from 0 (full left lock) to 4095 (right lock)
+not sure if left and right are inverted, need to check</t>
+  </si>
+  <si>
+    <t>calibration successful. Number represents the calibration mode that was carried out
+255 means calibration failed</t>
+  </si>
+  <si>
+    <t>raw value of centre reading (if calibrated)
+value = B2 + B3*256</t>
+  </si>
+  <si>
+    <t>centre angle (raw) = B1 + B2*256</t>
+  </si>
+  <si>
+    <t>0= max-min; 1= calibrate only min; 2=calibrate only max; 3=calibrate centre; 4=reset centre calibration
+suggested to do one at a time if you're doing it without a serial monitor</t>
   </si>
 </sst>
 </file>
@@ -758,7 +778,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -794,16 +814,23 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1105,10 +1132,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="S18" sqref="S18"/>
+      <selection pane="bottomLeft" activeCell="R82" sqref="R82:S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,23 +1161,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
       <c r="N1" s="9" t="s">
         <v>55</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>82</v>
@@ -1230,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
@@ -1245,7 +1272,7 @@
         <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>51</v>
@@ -1288,14 +1315,14 @@
         <v>22</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC10" s="23"/>
     </row>
@@ -1316,11 +1343,11 @@
         <v>22</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB11" s="24"/>
       <c r="AC11" s="23"/>
@@ -1330,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>80</v>
@@ -1342,11 +1369,11 @@
         <v>22</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB12" s="24"/>
       <c r="AC12" s="23"/>
@@ -1368,12 +1395,16 @@
         <v>22</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="19" t="s">
-        <v>136</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="R13" s="31"/>
       <c r="AB13" s="24"/>
       <c r="AC13" s="23"/>
     </row>
@@ -1382,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>69</v>
@@ -1394,11 +1425,11 @@
         <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -1406,10 +1437,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>4</v>
@@ -1418,10 +1449,10 @@
         <v>22</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -1434,7 +1465,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>4</v>
@@ -1443,10 +1474,10 @@
         <v>22</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1454,7 +1485,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>4</v>
@@ -1463,10 +1494,10 @@
         <v>22</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1474,16 +1505,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1491,16 +1522,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -1508,16 +1539,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1606,19 +1637,19 @@
         <v>61</v>
       </c>
       <c r="P34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q34" t="s">
+        <v>183</v>
+      </c>
+      <c r="R34" t="s">
         <v>185</v>
       </c>
-      <c r="R34" t="s">
-        <v>187</v>
-      </c>
       <c r="S34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="T34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1667,13 +1698,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G36" t="s">
         <v>19</v>
@@ -1682,13 +1713,13 @@
         <v>20</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P36" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q36" t="s">
         <v>176</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -1716,11 +1747,11 @@
         <v>57</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26" t="s">
@@ -1740,7 +1771,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
@@ -1749,19 +1780,19 @@
         <v>22</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P39" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q39" t="s">
         <v>183</v>
       </c>
-      <c r="Q39" t="s">
-        <v>185</v>
-      </c>
       <c r="R39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="S39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
@@ -1796,7 +1827,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>44</v>
       </c>
@@ -1815,12 +1846,12 @@
       <c r="N46" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P46" t="s">
-        <v>180</v>
-      </c>
-      <c r="R46" t="s">
-        <v>98</v>
-      </c>
+      <c r="P46" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
       <c r="AB46" s="6"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -1843,13 +1874,13 @@
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -1861,16 +1892,16 @@
         <v>61</v>
       </c>
       <c r="P50" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q50" t="s">
         <v>99</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>100</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>101</v>
-      </c>
-      <c r="S50" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1953,11 +1984,11 @@
         <v>61</v>
       </c>
       <c r="P54" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q54" s="26"/>
       <c r="R54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
@@ -1974,11 +2005,11 @@
         <v>4</v>
       </c>
       <c r="P55" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q55" s="26"/>
       <c r="R55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
@@ -1995,11 +2026,11 @@
         <v>4</v>
       </c>
       <c r="P56" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
@@ -2016,11 +2047,11 @@
         <v>4</v>
       </c>
       <c r="P57" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q57" s="26"/>
       <c r="R57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
@@ -2040,11 +2071,11 @@
         <v>57</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q58" s="26"/>
       <c r="R58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
@@ -2067,10 +2098,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -2079,13 +2110,13 @@
         <v>22</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P62" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q62" t="s">
         <v>170</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.25">
@@ -2093,10 +2124,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -2105,13 +2136,13 @@
         <v>22</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
@@ -2142,25 +2173,25 @@
       </c>
       <c r="O66" s="14"/>
       <c r="P66" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q66" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="Q66" s="12" t="s">
+      <c r="R66" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="R66" s="12" t="s">
-        <v>113</v>
-      </c>
       <c r="S66" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="T66" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="T66" s="12" t="s">
+      <c r="U66" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="U66" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="AB66" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC66" s="16"/>
     </row>
@@ -2169,27 +2200,27 @@
         <v>65</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D67" s="13" t="s">
         <v>69</v>
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="25" t="s">
+      <c r="P67" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="Q67" s="25"/>
-      <c r="R67" s="25" t="s">
+      <c r="S67" s="27"/>
+      <c r="T67" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S67" s="25"/>
-      <c r="T67" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="U67" s="25"/>
+      <c r="U67" s="27"/>
       <c r="AB67" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
@@ -2198,25 +2229,25 @@
         <v>66</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D68" s="13" t="s">
         <v>69</v>
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="25" t="s">
+      <c r="P68" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q68" s="27"/>
+      <c r="R68" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25" t="s">
+      <c r="S68" s="27"/>
+      <c r="T68" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="U68" s="25"/>
+      <c r="U68" s="27"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2225,25 +2256,25 @@
         <v>67</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>69</v>
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="25" t="s">
+      <c r="P69" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q69" s="27"/>
+      <c r="R69" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="Q69" s="25"/>
-      <c r="R69" s="25" t="s">
+      <c r="S69" s="27"/>
+      <c r="T69" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="S69" s="25"/>
-      <c r="T69" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="U69" s="25"/>
+      <c r="U69" s="27"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -2282,10 +2313,10 @@
       </c>
       <c r="O74" s="14"/>
       <c r="P74" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q74" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
@@ -2356,82 +2387,107 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:19" ht="150" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C82" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="M82" t="s">
+        <v>22</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P82" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q82" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="R82" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="S82" s="26"/>
+    </row>
+    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>94</v>
       </c>
@@ -2450,31 +2506,31 @@
         <v>96</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P98" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q98" t="s">
         <v>104</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>105</v>
       </c>
-      <c r="R98" t="s">
+      <c r="S98" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="T98" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="S98" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="T98" s="12" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
@@ -2482,31 +2538,31 @@
         <v>97</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E99" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P99" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q99" t="s">
         <v>104</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>105</v>
       </c>
-      <c r="R99" t="s">
+      <c r="S99" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="T99" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="S99" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="T99" s="12" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.25">
@@ -2529,19 +2585,19 @@
         <v>13</v>
       </c>
       <c r="N101" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P101" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q101" t="s">
         <v>104</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>105</v>
       </c>
-      <c r="R101" t="s">
-        <v>106</v>
-      </c>
       <c r="S101" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -3549,18 +3605,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
+  <mergeCells count="21">
+    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="Q13:R13"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3568,6 +3615,18 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P46:Q46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3618,7 +3677,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3646,7 +3705,7 @@
         <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
         <v>65</v>
@@ -3674,7 +3733,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -3688,24 +3747,24 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
         <v>137</v>
-      </c>
-      <c r="B10" t="s">
-        <v>138</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3713,7 +3772,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3732,15 +3791,15 @@
         <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
         <v>142</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -3748,16 +3807,16 @@
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3827,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of updates lol
SAS, BMS, TPS, Motor controller (dual) working. Yet to test motor controller (single), and more than 1 motor node connected at the same time
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="983" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D071626-7931-4AD7-A08F-9BED6556D84C}"/>
+  <xr:revisionPtr revIDLastSave="1050" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C215D7-1D10-4BFC-A3FD-0C6F68F824E5}"/>
   <bookViews>
-    <workbookView xWindow="-9930" yWindow="5415" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="3105" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
     <sheet name="Nodes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="210">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -320,9 +329,6 @@
   </si>
   <si>
     <t>Batt SOC (%) ;0-100%</t>
-  </si>
-  <si>
-    <t>FL: 0.4%/bit 0-100%</t>
   </si>
   <si>
     <t>FR</t>
@@ -496,9 +502,6 @@
     <t>Individual Wheel Throttles</t>
   </si>
   <si>
-    <t>Throttle Position = B0*0.4; 0-100%</t>
-  </si>
-  <si>
     <t>Battery Current(A) = -320 + (B3*256 + B2)*0.1</t>
   </si>
   <si>
@@ -526,9 +529,6 @@
     <t>fade (0: fade, 1: immediately change)</t>
   </si>
   <si>
-    <t>0: 100%front, 127: 50-50, 255: 100% rear</t>
-  </si>
-  <si>
     <t>HUD/ECU</t>
   </si>
   <si>
@@ -541,12 +541,6 @@
     <t>0: equal distribution between inner and outer wheel, 255: all power to outer wheel</t>
   </si>
   <si>
-    <t>scale wrt to steering angle; 0: none, 1: linear, 2: exponential, 3: logarithmic</t>
-  </si>
-  <si>
-    <t>scale wrt to acceleration/braking strength; 0: none, 1: linear, 2: exponential, 3: logarithmic</t>
-  </si>
-  <si>
     <t>Voltage Rail values</t>
   </si>
   <si>
@@ -559,21 +553,12 @@
     <t>Reverse (0:forward, 1:reverse)</t>
   </si>
   <si>
-    <t>mode (0: normal 1:eco 2:boost)</t>
-  </si>
-  <si>
     <t>when changed</t>
   </si>
   <si>
     <t>brake percent (%) B4*0.4; 0-100%. Could be calculated based on pressure</t>
   </si>
   <si>
-    <t>0 =  error, 1 = ok, 2 = estop pressed, 255 = offline</t>
-  </si>
-  <si>
-    <t>Front-Rear Differential Balance</t>
-  </si>
-  <si>
     <t>5V voltage(V) = B1/20 SCALING FACTOR MAY CHANGE</t>
   </si>
   <si>
@@ -593,11 +578,6 @@
   </si>
   <si>
     <t>HUD/SAS</t>
-  </si>
-  <si>
-    <t>angle(degrees) = ((B1*256 + B0)-2048)/130degrees
-raw data is from 0 (full left lock) to 4095 (right lock)
-not sure if left and right are inverted, need to check</t>
   </si>
   <si>
     <t>calibration successful. Number represents the calibration mode that was carried out
@@ -647,14 +627,106 @@
     <t>RR Reverse</t>
   </si>
   <si>
-    <t>Wheel speed (RPM) = (B1*256 + B0)/33; 0-1966RPM</t>
+    <r>
+      <t>Wheel speed (RPM) = (B1*256 + B0)/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; 0-1966RPM</t>
+    </r>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Phone Connected</t>
+  </si>
+  <si>
+    <t>0 = not connected
+1 = phone connected</t>
+  </si>
+  <si>
+    <t>Calibrate Throttle(?)</t>
+  </si>
+  <si>
+    <t>Throttle Position = B0*0.4; 0-100%
+raw data 0-250</t>
+  </si>
+  <si>
+    <t>Node Status Request</t>
+  </si>
+  <si>
+    <t>0 (all) or message requested (eg. 9 = BMS status requested)</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>*fade seems difficult to implement?</t>
+  </si>
+  <si>
+    <t>boost</t>
+  </si>
+  <si>
+    <t>eco</t>
+  </si>
+  <si>
+    <t>Front-Rear Differential Power Balance</t>
+  </si>
+  <si>
+    <t>0: equal distribution between front and rear wheels, 255: most power to rear wheels (scaled based on acceleration)</t>
+  </si>
+  <si>
+    <t>scale wrt to steering angle; 0: none, 1: linear, 2: exponential, 3: logarithmic
+(NOT IMPLEMENTED)</t>
+  </si>
+  <si>
+    <t>scale wrt to acceleration/braking strength; 0: none, 1: linear, 2: exponential, 3: logarithmic
+(NOT IMPLEMENTED)</t>
+  </si>
+  <si>
+    <t>**direction bit removed</t>
+  </si>
+  <si>
+    <t>NONE  = 0, THROTTLE_TIMED_OUT = 3, STEERING_TIMED_OUT = 4, WHEEL_SPEED_TIMED_OUT = 5</t>
+  </si>
+  <si>
+    <t>FL: 0.4%/bit 0-100%
+raw data 0-250</t>
+  </si>
+  <si>
+    <t>steering percentage = (B1*256+B0)
+raw data is from 0 (left lock) to 4095 (right lock). Centre is 2047-2048
+turning steering left means wheels turn left btw</t>
+  </si>
+  <si>
+    <t>calibrated steering percentage: 0 = left lock, 255 = right lock, 127-128 = centre</t>
+  </si>
+  <si>
+    <t>it's roughly 130 degrees per side, from the NARRco rack specs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +765,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -794,7 +880,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -830,12 +916,22 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,17 +939,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1155,9 +1242,9 @@
   <dimension ref="A1:AD301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,23 +1271,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
       <c r="N1" s="9" t="s">
         <v>52</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>79</v>
@@ -1280,22 +1367,22 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="32" t="s">
-        <v>189</v>
+      <c r="N6" s="25" t="s">
+        <v>180</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="AB6" s="6"/>
     </row>
@@ -1304,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>22</v>
@@ -1313,14 +1400,14 @@
         <v>4</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>189</v>
+        <v>179</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>180</v>
       </c>
       <c r="O7" s="21"/>
-      <c r="P7" s="33" t="s">
-        <v>191</v>
+      <c r="P7" s="26" t="s">
+        <v>182</v>
       </c>
       <c r="AB7" s="24"/>
       <c r="AC7" s="23"/>
@@ -1334,6 +1421,21 @@
       <c r="B9">
         <v>7</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>196</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="10" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19">
@@ -1349,11 +1451,14 @@
         <v>22</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>173</v>
+        <v>129</v>
+      </c>
+      <c r="Q10" s="28" t="s">
+        <v>205</v>
       </c>
       <c r="AB10" s="22"/>
       <c r="AC10" s="23"/>
@@ -1375,11 +1480,11 @@
         <v>22</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB11" s="24"/>
       <c r="AC11" s="23"/>
@@ -1389,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>77</v>
@@ -1401,11 +1506,11 @@
         <v>22</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB12" s="24"/>
       <c r="AC12" s="23"/>
@@ -1427,16 +1532,16 @@
         <v>22</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q13" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="R13" s="28"/>
+        <v>129</v>
+      </c>
+      <c r="Q13" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="R13" s="32"/>
       <c r="AB13" s="24"/>
       <c r="AC13" s="23"/>
     </row>
@@ -1445,7 +1550,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>66</v>
@@ -1457,11 +1562,11 @@
         <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -1469,10 +1574,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>4</v>
@@ -1481,10 +1586,10 @@
         <v>22</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -1497,7 +1602,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>4</v>
@@ -1506,10 +1611,10 @@
         <v>22</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1517,7 +1622,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>4</v>
@@ -1526,10 +1631,10 @@
         <v>22</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1537,16 +1642,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1554,16 +1659,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -1571,16 +1676,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1646,7 +1751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1668,20 +1773,20 @@
       <c r="N34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P34" t="s">
-        <v>149</v>
+      <c r="P34" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="Q34" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="R34" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="S34" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="T34" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1730,16 +1835,16 @@
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>19</v>
@@ -1748,13 +1853,16 @@
         <v>20</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="P36" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="Q36" t="s">
-        <v>170</v>
+        <v>198</v>
+      </c>
+      <c r="R36" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -1781,18 +1889,18 @@
       <c r="N38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P38" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27" t="s">
+      <c r="P38" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="U38" s="27"/>
+      <c r="U38" s="30"/>
       <c r="V38" t="s">
         <v>94</v>
       </c>
@@ -1806,7 +1914,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>11</v>
@@ -1815,19 +1923,19 @@
         <v>22</v>
       </c>
       <c r="N39" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="P39" t="s">
         <v>167</v>
       </c>
-      <c r="P39" t="s">
-        <v>175</v>
-      </c>
       <c r="Q39" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="R39" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="S39" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
@@ -1862,7 +1970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>44</v>
       </c>
@@ -1881,12 +1989,16 @@
       <c r="N46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P46" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q46" s="26"/>
-      <c r="R46" s="25"/>
-      <c r="S46" s="25"/>
+      <c r="P46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q46" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="R46" s="31"/>
+      <c r="S46" t="s">
+        <v>209</v>
+      </c>
       <c r="AB46" s="6"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -1904,18 +2016,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:29" ht="30" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -1926,29 +2038,29 @@
       <c r="N50" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q50" t="s">
         <v>95</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>96</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>97</v>
       </c>
-      <c r="S50" t="s">
-        <v>98</v>
-      </c>
       <c r="T50" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="U50" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="V50" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="W50" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2030,12 +2142,15 @@
       <c r="N54" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P54" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q54" s="27"/>
-      <c r="R54" t="s">
-        <v>153</v>
+      <c r="P54" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q54" s="30"/>
+      <c r="R54" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="T54" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
@@ -2051,12 +2166,12 @@
       <c r="E55" t="s">
         <v>4</v>
       </c>
-      <c r="P55" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q55" s="27"/>
-      <c r="R55" t="s">
-        <v>153</v>
+      <c r="P55" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q55" s="30"/>
+      <c r="R55" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
@@ -2072,12 +2187,12 @@
       <c r="E56" t="s">
         <v>4</v>
       </c>
-      <c r="P56" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q56" s="27"/>
-      <c r="R56" t="s">
-        <v>153</v>
+      <c r="P56" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
@@ -2093,12 +2208,12 @@
       <c r="E57" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q57" s="27"/>
-      <c r="R57" t="s">
-        <v>153</v>
+      <c r="P57" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q57" s="30"/>
+      <c r="R57" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
@@ -2117,12 +2232,12 @@
       <c r="N58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P58" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q58" s="27"/>
-      <c r="R58" t="s">
-        <v>153</v>
+      <c r="P58" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q58" s="30"/>
+      <c r="R58" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
@@ -2140,15 +2255,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:29" ht="90" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>60</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -2157,24 +2272,24 @@
         <v>22</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P62" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="2:29" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="2:29" ht="105" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -2183,13 +2298,13 @@
         <v>22</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P63" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>165</v>
+        <v>201</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.25">
@@ -2220,25 +2335,25 @@
       </c>
       <c r="O66" s="14"/>
       <c r="P66" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q66" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="Q66" s="12" t="s">
+      <c r="R66" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="R66" s="12" t="s">
-        <v>109</v>
-      </c>
       <c r="S66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="T66" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="T66" s="12" t="s">
+      <c r="U66" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="U66" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="AB66" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC66" s="16"/>
     </row>
@@ -2247,27 +2362,27 @@
         <v>65</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D67" s="13" t="s">
         <v>66</v>
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="29" t="s">
+      <c r="P67" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q67" s="33"/>
+      <c r="R67" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="Q67" s="29"/>
-      <c r="R67" s="29" t="s">
+      <c r="S67" s="33"/>
+      <c r="T67" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="S67" s="29"/>
-      <c r="T67" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="U67" s="29"/>
+      <c r="U67" s="33"/>
       <c r="AB67" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
@@ -2276,25 +2391,25 @@
         <v>66</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D68" s="13" t="s">
         <v>66</v>
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="29" t="s">
+      <c r="P68" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q68" s="33"/>
+      <c r="R68" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="Q68" s="29"/>
-      <c r="R68" s="29" t="s">
+      <c r="S68" s="33"/>
+      <c r="T68" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="S68" s="29"/>
-      <c r="T68" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="U68" s="29"/>
+      <c r="U68" s="33"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2303,25 +2418,25 @@
         <v>67</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>66</v>
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="29" t="s">
+      <c r="P69" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q69" s="33"/>
+      <c r="R69" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="Q69" s="29"/>
-      <c r="R69" s="29" t="s">
+      <c r="S69" s="33"/>
+      <c r="T69" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="S69" s="29"/>
-      <c r="T69" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="U69" s="29"/>
+      <c r="U69" s="33"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -2360,10 +2475,10 @@
       </c>
       <c r="O74" s="14"/>
       <c r="P74" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q74" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
@@ -2439,15 +2554,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:19" ht="135" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E82" t="s">
         <v>9</v>
@@ -2459,20 +2574,26 @@
         <v>53</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="R82" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="S82" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="R82" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="S82" s="30"/>
     </row>
     <row r="83" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>81</v>
       </c>
+      <c r="C83" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="84" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B84">
@@ -2543,6 +2664,9 @@
       <c r="B97">
         <v>95</v>
       </c>
+      <c r="S97" t="s">
+        <v>197</v>
+      </c>
       <c r="AB97" s="6"/>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
@@ -2553,31 +2677,31 @@
         <v>96</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P98" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q98" t="s">
         <v>100</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>101</v>
       </c>
-      <c r="R98" t="s">
+      <c r="S98" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="T98" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="S98" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="T98" s="12" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
@@ -2585,31 +2709,31 @@
         <v>97</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P99" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q99" t="s">
         <v>100</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>101</v>
       </c>
-      <c r="R99" t="s">
+      <c r="S99" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="T99" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="S99" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="T99" s="12" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.25">
@@ -2632,19 +2756,19 @@
         <v>13</v>
       </c>
       <c r="N101" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P101" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q101" t="s">
         <v>100</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>101</v>
       </c>
-      <c r="R101" t="s">
-        <v>102</v>
-      </c>
       <c r="S101" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -2703,82 +2827,94 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>189</v>
+      </c>
       <c r="B114">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C114" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P114" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>126</v>
       </c>
@@ -3653,12 +3789,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P46:Q46"/>
     <mergeCell ref="R82:S82"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="R67:S67"/>
@@ -3674,6 +3804,12 @@
     <mergeCell ref="P58:Q58"/>
     <mergeCell ref="P68:Q68"/>
     <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="Q46:R46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3706,15 +3842,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3724,7 +3860,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3752,7 +3888,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
         <v>62</v>
@@ -3780,7 +3916,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -3794,24 +3930,24 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
         <v>131</v>
-      </c>
-      <c r="B10" t="s">
-        <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,7 +3955,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3838,15 +3974,15 @@
         <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
         <v>136</v>
-      </c>
-      <c r="B17" t="s">
-        <v>137</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -3854,16 +3990,16 @@
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3874,7 +4010,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix: bms status error
bms was outputting voltage as its status
</commit_message>
<xml_diff>
--- a/Notes/CAN Bus Messages.xlsx
+++ b/Notes/CAN Bus Messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam_canbus/Notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Documents\GitHub\evam_canbus\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1050" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C215D7-1D10-4BFC-A3FD-0C6F68F824E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0445BC2-4712-42A5-97B1-8C96C9BB8851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="3105" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1354" yWindow="377" windowWidth="19346" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -559,9 +559,6 @@
     <t>brake percent (%) B4*0.4; 0-100%. Could be calculated based on pressure</t>
   </si>
   <si>
-    <t>5V voltage(V) = B1/20 SCALING FACTOR MAY CHANGE</t>
-  </si>
-  <si>
     <t>12V voltage(V) = B2/10 SCALING FACTOR MAY CHANGE</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>it's roughly 130 degrees per side, from the NARRco rack specs</t>
+  </si>
+  <si>
+    <t>5V voltage(V) = B1/36 UNCALIBRATED</t>
   </si>
 </sst>
 </file>
@@ -880,7 +880,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -907,7 +907,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -923,20 +922,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1241,27 +1239,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P46" sqref="P46"/>
+      <selection pane="bottomLeft" activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="30" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="22.7109375" customWidth="1"/>
-    <col min="17" max="23" width="20.5703125" customWidth="1"/>
-    <col min="28" max="28" width="100.140625" style="5" customWidth="1"/>
-    <col min="29" max="29" width="2.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.84375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.3046875" customWidth="1"/>
+    <col min="14" max="14" width="13.69140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="1.53515625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="22.69140625" customWidth="1"/>
+    <col min="17" max="23" width="20.53515625" customWidth="1"/>
+    <col min="28" max="28" width="100.15234375" style="5" customWidth="1"/>
+    <col min="29" max="29" width="2.53515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,17 +1269,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
       <c r="N1" s="9" t="s">
         <v>52</v>
       </c>
@@ -1321,7 +1319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1335,7 +1333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1346,7 +1344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1354,7 +1352,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1362,7 +1360,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1373,179 +1371,179 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="AB6" s="6"/>
+    </row>
+    <row r="7" spans="1:30" s="18" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B7" s="18">
+        <v>5</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="AB6" s="6"/>
-    </row>
-    <row r="7" spans="1:30" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="19">
-        <v>5</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="N7" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="23"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="22"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="P9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="18">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="19" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="Q10" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="23"/>
-    </row>
-    <row r="11" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19">
+      <c r="Q10" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="22"/>
+    </row>
+    <row r="11" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="18">
         <v>9</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="19" t="s">
+      <c r="O11" s="20"/>
+      <c r="P11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="23"/>
-    </row>
-    <row r="12" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="19">
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="22"/>
+    </row>
+    <row r="12" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="18">
         <v>10</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O12" s="21"/>
-      <c r="P12" s="19" t="s">
+      <c r="O12" s="20"/>
+      <c r="P12" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="23"/>
-    </row>
-    <row r="13" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19">
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="22"/>
+    </row>
+    <row r="13" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="18">
         <v>11</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="19" t="s">
+      <c r="M13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="19" t="s">
+      <c r="O13" s="20"/>
+      <c r="P13" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="Q13" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="R13" s="32"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="23"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Q13" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="R13" s="29"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="22"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1555,21 +1553,21 @@
       <c r="D14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="N14" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O14" s="21"/>
-      <c r="P14" s="19" t="s">
+      <c r="O14" s="20"/>
+      <c r="P14" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>13</v>
       </c>
@@ -1579,171 +1577,171 @@
       <c r="D15" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="20" t="s">
+      <c r="N15" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P15" s="19" t="s">
+      <c r="P15" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P17" s="19" t="s">
+      <c r="P17" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="M18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N18" s="20" t="s">
+      <c r="N18" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P18" s="19" t="s">
+      <c r="P18" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M19" s="19" t="s">
+      <c r="M19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="N19" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P20" s="19" t="s">
+      <c r="P20" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M21" s="19" t="s">
+      <c r="M21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="20" t="s">
+      <c r="N21" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B33">
         <v>31</v>
       </c>
@@ -1751,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1774,16 +1772,16 @@
         <v>58</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q34" t="s">
+        <v>168</v>
+      </c>
+      <c r="R34" t="s">
+        <v>170</v>
+      </c>
+      <c r="S34" t="s">
         <v>169</v>
-      </c>
-      <c r="R34" t="s">
-        <v>171</v>
-      </c>
-      <c r="S34" t="s">
-        <v>170</v>
       </c>
       <c r="T34" t="s">
         <v>166</v>
@@ -1793,7 +1791,7 @@
       </c>
       <c r="AB34" s="6"/>
     </row>
-    <row r="35" spans="1:30" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" s="12" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B35" s="12">
         <v>33</v>
       </c>
@@ -1830,7 +1828,7 @@
       </c>
       <c r="AC35" s="16"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B36">
         <v>34</v>
       </c>
@@ -1843,13 +1841,13 @@
       <c r="E36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="18" t="s">
         <v>20</v>
       </c>
       <c r="N36" s="3" t="s">
@@ -1859,18 +1857,18 @@
         <v>164</v>
       </c>
       <c r="Q36" t="s">
+        <v>197</v>
+      </c>
+      <c r="R36" t="s">
         <v>198</v>
       </c>
-      <c r="R36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B38">
         <v>36</v>
       </c>
@@ -1889,18 +1887,18 @@
       <c r="N38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P38" s="30" t="s">
+      <c r="P38" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30" t="s">
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30" t="s">
+      <c r="S38" s="28"/>
+      <c r="T38" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="U38" s="30"/>
+      <c r="U38" s="28"/>
       <c r="V38" t="s">
         <v>94</v>
       </c>
@@ -1909,7 +1907,7 @@
       </c>
       <c r="AB38" s="6"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B39">
         <v>37</v>
       </c>
@@ -1926,51 +1924,51 @@
         <v>162</v>
       </c>
       <c r="P39" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>168</v>
+      </c>
+      <c r="R39" t="s">
         <v>167</v>
       </c>
-      <c r="Q39" t="s">
-        <v>169</v>
-      </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>168</v>
       </c>
-      <c r="S39" t="s">
-        <v>169</v>
-      </c>
       <c r="AB39" s="6"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="AB40" s="6"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46">
         <v>44</v>
       </c>
@@ -1990,33 +1988,33 @@
         <v>58</v>
       </c>
       <c r="P46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q46" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="R46" s="27"/>
+      <c r="S46" t="s">
         <v>208</v>
       </c>
-      <c r="Q46" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="R46" s="31"/>
-      <c r="S46" t="s">
-        <v>209</v>
-      </c>
       <c r="AB46" s="6"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:29" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B50">
         <v>48</v>
       </c>
@@ -2039,7 +2037,7 @@
         <v>58</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q50" t="s">
         <v>95</v>
@@ -2051,19 +2049,19 @@
         <v>97</v>
       </c>
       <c r="T50" t="s">
+        <v>183</v>
+      </c>
+      <c r="U50" t="s">
         <v>184</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>185</v>
       </c>
-      <c r="V50" t="s">
+      <c r="W50" t="s">
         <v>186</v>
       </c>
-      <c r="W50" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B51" s="12">
         <v>49</v>
       </c>
@@ -2084,7 +2082,7 @@
       <c r="AB51" s="17"/>
       <c r="AC51" s="16"/>
     </row>
-    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B52" s="12">
         <v>50</v>
       </c>
@@ -2105,7 +2103,7 @@
       <c r="AB52" s="17"/>
       <c r="AC52" s="16"/>
     </row>
-    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B53" s="12">
         <v>51</v>
       </c>
@@ -2126,7 +2124,7 @@
       <c r="AB53" s="17"/>
       <c r="AC53" s="16"/>
     </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B54">
         <v>52</v>
       </c>
@@ -2142,18 +2140,18 @@
       <c r="N54" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="P54" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q54" s="30"/>
-      <c r="R54" s="27" t="s">
+      <c r="P54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q54" s="28"/>
+      <c r="R54" s="26" t="s">
         <v>151</v>
       </c>
       <c r="T54" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B55">
         <v>53</v>
       </c>
@@ -2166,15 +2164,15 @@
       <c r="E55" t="s">
         <v>4</v>
       </c>
-      <c r="P55" s="30" t="s">
+      <c r="P55" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="27" t="s">
+      <c r="Q55" s="28"/>
+      <c r="R55" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B56">
         <v>54</v>
       </c>
@@ -2187,15 +2185,15 @@
       <c r="E56" t="s">
         <v>4</v>
       </c>
-      <c r="P56" s="30" t="s">
+      <c r="P56" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="Q56" s="30"/>
-      <c r="R56" s="27" t="s">
+      <c r="Q56" s="28"/>
+      <c r="R56" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B57">
         <v>55</v>
       </c>
@@ -2208,15 +2206,15 @@
       <c r="E57" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="30" t="s">
+      <c r="P57" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="27" t="s">
+      <c r="Q57" s="28"/>
+      <c r="R57" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B58">
         <v>56</v>
       </c>
@@ -2232,30 +2230,30 @@
       <c r="N58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P58" s="30" t="s">
+      <c r="P58" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="Q58" s="30"/>
-      <c r="R58" s="27" t="s">
+      <c r="Q58" s="28"/>
+      <c r="R58" s="26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B59">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B60">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B61">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:29" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="B62">
         <v>60</v>
       </c>
@@ -2278,15 +2276,15 @@
         <v>160</v>
       </c>
       <c r="Q62" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="2:29" ht="105" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="2:29" ht="87.45" x14ac:dyDescent="0.4">
       <c r="B63">
         <v>61</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>157</v>
@@ -2301,23 +2299,23 @@
         <v>158</v>
       </c>
       <c r="P63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B64">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="12" t="s">
         <v>76</v>
       </c>
@@ -2357,7 +2355,7 @@
       </c>
       <c r="AC66" s="16"/>
     </row>
-    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B67" s="12">
         <v>65</v>
       </c>
@@ -2369,24 +2367,24 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="33" t="s">
+      <c r="P67" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="Q67" s="33"/>
-      <c r="R67" s="33" t="s">
+      <c r="Q67" s="30"/>
+      <c r="R67" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="S67" s="33"/>
-      <c r="T67" s="33" t="s">
+      <c r="S67" s="30"/>
+      <c r="T67" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="U67" s="33"/>
+      <c r="U67" s="30"/>
       <c r="AB67" s="17" t="s">
         <v>118</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
-    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B68" s="12">
         <v>66</v>
       </c>
@@ -2398,22 +2396,22 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="33" t="s">
+      <c r="P68" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="Q68" s="33"/>
-      <c r="R68" s="33" t="s">
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="S68" s="33"/>
-      <c r="T68" s="33" t="s">
+      <c r="S68" s="30"/>
+      <c r="T68" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="U68" s="33"/>
+      <c r="U68" s="30"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
-    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B69" s="12">
         <v>67</v>
       </c>
@@ -2425,42 +2423,42 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="33" t="s">
+      <c r="P69" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="Q69" s="33"/>
-      <c r="R69" s="33" t="s">
+      <c r="Q69" s="30"/>
+      <c r="R69" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="S69" s="33"/>
-      <c r="T69" s="33" t="s">
+      <c r="S69" s="30"/>
+      <c r="T69" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="U69" s="33"/>
+      <c r="U69" s="30"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B74" s="12">
         <v>72</v>
       </c>
@@ -2483,7 +2481,7 @@
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
     </row>
-    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B75" s="12">
         <v>73</v>
       </c>
@@ -2500,7 +2498,7 @@
       <c r="AB75" s="17"/>
       <c r="AC75" s="16"/>
     </row>
-    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B76" s="12">
         <v>74</v>
       </c>
@@ -2517,7 +2515,7 @@
       <c r="AB76" s="17"/>
       <c r="AC76" s="16"/>
     </row>
-    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B77" s="12">
         <v>75</v>
       </c>
@@ -2534,35 +2532,35 @@
       <c r="AB77" s="17"/>
       <c r="AC77" s="16"/>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:19" ht="135" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:19" ht="102" x14ac:dyDescent="0.4">
       <c r="B82">
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="E82" t="s">
         <v>9</v>
@@ -2574,102 +2572,102 @@
         <v>53</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q82" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R82" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="R82" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="S82" s="30"/>
-    </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S82" s="28"/>
+    </row>
+    <row r="83" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B83">
         <v>81</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B97">
         <v>95</v>
       </c>
       <c r="S97" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AB97" s="6"/>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -2682,7 +2680,7 @@
       <c r="D98" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E98" s="18" t="s">
+      <c r="E98" t="s">
         <v>135</v>
       </c>
       <c r="N98" s="3" t="s">
@@ -2697,14 +2695,14 @@
       <c r="R98" t="s">
         <v>101</v>
       </c>
-      <c r="S98" s="19" t="s">
+      <c r="S98" s="18" t="s">
         <v>156</v>
       </c>
       <c r="T98" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B99">
         <v>97</v>
       </c>
@@ -2729,20 +2727,20 @@
       <c r="R99" t="s">
         <v>101</v>
       </c>
-      <c r="S99" s="19" t="s">
+      <c r="S99" s="18" t="s">
         <v>156</v>
       </c>
       <c r="T99" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B100">
         <v>98</v>
       </c>
-      <c r="S100" s="19"/>
-    </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S100" s="18"/>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B101">
         <v>99</v>
       </c>
@@ -2767,499 +2765,499 @@
       <c r="R101" t="s">
         <v>101</v>
       </c>
-      <c r="S101" s="19" t="s">
+      <c r="S101" s="18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B102">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B103">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B104">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B105">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B106">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B107">
         <v>105</v>
       </c>
       <c r="AB107" s="6"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B108">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B109">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B110">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B111">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B112">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B113">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B114">
         <v>112</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>22</v>
       </c>
       <c r="P114" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B115">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B116">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B117">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B118">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B119">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B120">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B121">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B122">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B123">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B124">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B125">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B126">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B127">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B128">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B129">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B130">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B131">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B132">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B133">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B134">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B135">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B136">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B137">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B138">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B139">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B140">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B141">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B142">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B143">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B144">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B145">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B146">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B147">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B148">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B149">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B150">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B151">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B152">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B153">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B154">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B155">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B156">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B157">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B158">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B159">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B160">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B161">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B162">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B163">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B164">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B165">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B166">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B167">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B168">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B169">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B170">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B171">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B172">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B173">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B174">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B175">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B176">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B177">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B178">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B179">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B180">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B181">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B182">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B183">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B184">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B185">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B186">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B187">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B188">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B189">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B190">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B191">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B192">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B193">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B194">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B195">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B196">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
         <v>57</v>
       </c>
@@ -3267,528 +3265,534 @@
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B198">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B199">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B200">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B201">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B202">
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B203">
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B204">
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B205">
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B206">
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B207">
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B208">
         <v>206</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B209">
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B210">
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B211">
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B212">
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B213">
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B214">
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B215">
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B216">
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B217">
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B218">
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B219">
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B220">
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B221">
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B222">
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B223">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B224">
         <v>222</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B225">
         <v>223</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B226">
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B227">
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B228">
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B229">
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B230">
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B231">
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B232">
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B233">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B234">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B235">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B236">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B237">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B238">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B239">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B240">
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B241">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B242">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B243">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B244">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B245">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B246">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B247">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B248">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B249">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B250">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B251">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B252">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B253">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B254">
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B255">
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B256">
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B257">
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B258">
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B259">
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B260">
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B261">
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B262">
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B263">
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B264">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B265">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B266">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B267">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B268">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B269">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B270">
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B271">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B272">
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B273">
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B274">
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B275">
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B276">
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B277">
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B278">
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B279">
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B280">
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B281">
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B282">
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B283">
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B284">
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B285">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B286">
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B287">
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B288">
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B289">
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B290">
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B291">
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B292">
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B293">
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B294">
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B295">
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B296">
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B297">
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B298">
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B299">
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B300">
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B301">
         <v>299</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="Q46:R46"/>
     <mergeCell ref="R82:S82"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="R67:S67"/>
@@ -3804,12 +3808,6 @@
     <mergeCell ref="P58:Q58"/>
     <mergeCell ref="P68:Q68"/>
     <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="Q46:R46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3833,26 +3831,26 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.84375" customWidth="1"/>
+    <col min="3" max="3" width="51.3828125" customWidth="1"/>
+    <col min="4" max="4" width="48.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:7" ht="19.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3866,7 +3864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="105.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="102.45" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3880,7 +3878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -3894,7 +3892,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3908,7 +3906,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3922,7 +3920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3936,7 +3934,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -3950,7 +3948,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3958,7 +3956,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3966,7 +3964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3977,7 +3975,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -3988,7 +3986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -4002,7 +4000,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>13</v>
       </c>

</xml_diff>